<commit_message>
Work from 7/11-7/13 [1]
</commit_message>
<xml_diff>
--- a/resources/documents/placeholder_cut.xlsx
+++ b/resources/documents/placeholder_cut.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25428"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/BlameJack/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECED6296-D795-5749-B947-E815A737FD81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{58996C38-8E5C-44C1-B96C-FD58C20438B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="540" windowWidth="29320" windowHeight="18780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,10 @@
     <t>Output Data</t>
   </si>
   <si>
-    <t>Quote</t>
+    <t>Tool</t>
+  </si>
+  <si>
+    <t>Material</t>
   </si>
   <si>
     <t>Part Length</t>
@@ -52,28 +55,25 @@
     <t>Part Height</t>
   </si>
   <si>
+    <t>Volume</t>
+  </si>
+  <si>
     <t>Precision</t>
   </si>
   <si>
-    <t>Material</t>
-  </si>
-  <si>
-    <t>Volume</t>
-  </si>
-  <si>
     <t>Volume to Remove</t>
   </si>
   <si>
+    <t>Estimated FR Ratio</t>
+  </si>
+  <si>
+    <t>Estimated Error</t>
+  </si>
+  <si>
+    <t>Estimated Average Cut Rate</t>
+  </si>
+  <si>
     <t>Estimated Time Costs</t>
-  </si>
-  <si>
-    <t>Estimated FR Ratio</t>
-  </si>
-  <si>
-    <t>Estimated Error</t>
-  </si>
-  <si>
-    <t>Estimated Average Cut Rate</t>
   </si>
 </sst>
 </file>
@@ -81,9 +81,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,16 +164,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -183,7 +181,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,28 +497,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="164" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="164" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -539,42 +536,42 @@
       <c r="K1" s="6"/>
       <c r="L1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>